<commit_message>
maj schema de la carte robot
</commit_message>
<xml_diff>
--- a/Electronique/Carte Robot (base sur un Teensy 3.6)/Brochage Teensy 3.6.xlsx
+++ b/Electronique/Carte Robot (base sur un Teensy 3.6)/Brochage Teensy 3.6.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git folder\my_robot\Electronique\Carte Robot (base sur un Teensy 3.6)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git Folder\my_robot\Electronique\Carte Robot (base sur un Teensy 3.6)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46AC1976-8B8E-4F9B-9E94-C20C09E009E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9E87DD-F949-45BA-B95A-68DC7F50F486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Teensy 3.6" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>Labels</t>
   </si>
@@ -35,6 +35,24 @@
   </si>
   <si>
     <t>Fonction</t>
+  </si>
+  <si>
+    <t>A21</t>
+  </si>
+  <si>
+    <t>GND</t>
+  </si>
+  <si>
+    <t>Vbat</t>
+  </si>
+  <si>
+    <t>Vin</t>
+  </si>
+  <si>
+    <t>5V</t>
+  </si>
+  <si>
+    <t>3.3V</t>
   </si>
 </sst>
 </file>
@@ -66,7 +84,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -76,6 +94,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -92,18 +116,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O18" sqref="O18"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -449,15 +481,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE46DD2A-558F-4BCF-AF33-60DC5A92DC6E}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="8.7109375" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" style="4" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -476,78 +508,151 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C3" s="3" t="s">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>1</v>
       </c>
+      <c r="D3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C4" s="3"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="5"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C5" s="3"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C6" s="3"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C7" s="3"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="5"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C8" s="3"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="3"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="5"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C10" s="3"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="5"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C11" s="3"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="5"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C12" s="3"/>
+      <c r="B12" s="6"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="5"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C13" s="3"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="5"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C14" s="3"/>
+      <c r="B14" s="6"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="5"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C15" s="3"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C16" s="3"/>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" s="3"/>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" s="3"/>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" s="3"/>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20" s="3"/>
-    </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21" s="3"/>
-    </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C22" s="3"/>
-    </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C23" s="3"/>
-    </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C24" s="3"/>
-    </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C25" s="3"/>
-    </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C26" s="3"/>
+      <c r="B16" s="6"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="4"/>
+      <c r="D17" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="6"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="5"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" s="6"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20" s="6"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="5"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" s="6"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="5"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" s="6"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="5"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" s="6"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="5"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" s="6"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="5"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" s="6"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="5"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" s="6"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
ajout driver schema de la carte
</commit_message>
<xml_diff>
--- a/Electronique/Carte Robot (base sur un Teensy 3.6)/Brochage Teensy 3.6.xlsx
+++ b/Electronique/Carte Robot (base sur un Teensy 3.6)/Brochage Teensy 3.6.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git Folder\my_robot\Electronique\Carte Robot (base sur un Teensy 3.6)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9E87DD-F949-45BA-B95A-68DC7F50F486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F259302B-50BE-439B-9243-F3ED9B842C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
   <si>
     <t>Labels</t>
   </si>
@@ -53,13 +53,28 @@
   </si>
   <si>
     <t>3.3V</t>
+  </si>
+  <si>
+    <t>AGND</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>A22</t>
+  </si>
+  <si>
+    <t>STEP_G</t>
+  </si>
+  <si>
+    <t>STEP_D</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -79,6 +94,13 @@
       <b/>
       <sz val="18"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -116,7 +138,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -124,9 +146,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -136,6 +155,10 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,7 +489,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
@@ -482,7 +505,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,13 +534,13 @@
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E3" t="s">
@@ -525,134 +548,185 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="6"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="6"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="5"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="6"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="4">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="6"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="4">
+        <v>22</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="6"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="5"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="4">
+        <v>21</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="6"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="5"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="4">
+        <v>20</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="6"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="4">
+        <v>19</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="6"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="5"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="4">
+        <v>18</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="6"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="4">
+        <v>17</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="6"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="4">
+        <v>16</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="6"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="5"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="4">
+        <v>15</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="6"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="5"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="4">
+        <v>14</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="6"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="5"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="4">
+        <v>13</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="5" t="s">
+      <c r="C17" s="8"/>
+      <c r="D17" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="7" t="s">
+      <c r="E17" s="6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B18" s="6"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="5"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B19" s="6"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="5" t="s">
+      <c r="B19" s="5"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E19" t="s">
-        <v>5</v>
-      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B20" s="6"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="5"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="4">
+        <v>39</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B21" s="6"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="5"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="4">
+        <v>38</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B22" s="6"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="5"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="4">
+        <v>37</v>
+      </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B23" s="6"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="5"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="4">
+        <v>36</v>
+      </c>
+      <c r="E23" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B24" s="6"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="5"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="4">
+        <v>35</v>
+      </c>
+      <c r="E24" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B25" s="6"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="4">
+        <v>34</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B26" s="6"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="4">
+        <v>33</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
ajouts des connecteurs pour l'uart
</commit_message>
<xml_diff>
--- a/Electronique/Carte Robot (base sur un Teensy 3.6)/Brochage Teensy 3.6.xlsx
+++ b/Electronique/Carte Robot (base sur un Teensy 3.6)/Brochage Teensy 3.6.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git Folder\my_robot\Electronique\Carte Robot (base sur un Teensy 3.6)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F259302B-50BE-439B-9243-F3ED9B842C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5757412D-B521-4AC0-AFA9-4B48D403A081}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>Labels</t>
   </si>
@@ -68,6 +68,24 @@
   </si>
   <si>
     <t>STEP_D</t>
+  </si>
+  <si>
+    <t>RX3</t>
+  </si>
+  <si>
+    <t>RX2</t>
+  </si>
+  <si>
+    <t>TX3 (AX12)</t>
+  </si>
+  <si>
+    <t>TX2 (XL320)</t>
+  </si>
+  <si>
+    <t>RX1 (Lidar)</t>
+  </si>
+  <si>
+    <t>TX1 (Lidar)</t>
   </si>
 </sst>
 </file>
@@ -100,7 +118,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -489,7 +506,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
@@ -505,14 +522,16 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
     <col min="2" max="2" width="8.7109375" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" customWidth="1"/>
     <col min="4" max="4" width="8.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -548,21 +567,33 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="5"/>
+      <c r="A4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0</v>
+      </c>
       <c r="C4" s="8"/>
       <c r="D4" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="5"/>
+      <c r="A5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
       <c r="C5" s="8"/>
       <c r="D5" s="4" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="5"/>
+      <c r="B6" s="4">
+        <v>2</v>
+      </c>
       <c r="C6" s="8"/>
       <c r="D6" s="4">
         <v>23</v>
@@ -572,70 +603,102 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="5"/>
+      <c r="B7" s="4">
+        <v>3</v>
+      </c>
       <c r="C7" s="8"/>
       <c r="D7" s="4">
         <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="5"/>
+      <c r="B8" s="4">
+        <v>4</v>
+      </c>
       <c r="C8" s="8"/>
       <c r="D8" s="4">
         <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B9" s="5"/>
+      <c r="B9" s="4">
+        <v>5</v>
+      </c>
       <c r="C9" s="8"/>
       <c r="D9" s="4">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B10" s="5"/>
+      <c r="B10" s="4">
+        <v>6</v>
+      </c>
       <c r="C10" s="8"/>
       <c r="D10" s="4">
         <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="5"/>
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="4">
+        <v>7</v>
+      </c>
       <c r="C11" s="8"/>
       <c r="D11" s="4">
         <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="5"/>
+      <c r="A12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="4">
+        <v>8</v>
+      </c>
       <c r="C12" s="8"/>
       <c r="D12" s="4">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="5"/>
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13" s="4">
+        <v>9</v>
+      </c>
       <c r="C13" s="8"/>
       <c r="D13" s="4">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B14" s="5"/>
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" s="4">
+        <v>10</v>
+      </c>
       <c r="C14" s="8"/>
       <c r="D14" s="4">
         <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B15" s="5"/>
+      <c r="B15" s="4">
+        <v>11</v>
+      </c>
       <c r="C15" s="8"/>
       <c r="D15" s="4">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B16" s="5"/>
+      <c r="B16" s="4">
+        <v>12</v>
+      </c>
       <c r="C16" s="8"/>
       <c r="D16" s="4">
         <v>13</v>

</xml_diff>

<commit_message>
adaptateur servo Dynamixel + connecteur SPI
</commit_message>
<xml_diff>
--- a/Electronique/Carte Robot (base sur un Teensy 3.6)/Brochage Teensy 3.6.xlsx
+++ b/Electronique/Carte Robot (base sur un Teensy 3.6)/Brochage Teensy 3.6.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git Folder\my_robot\Electronique\Carte Robot (base sur un Teensy 3.6)\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git folder\my_robot\Electronique\Carte Robot (base sur un Teensy 3.6)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B7BB69C-8BCC-43C1-8372-DCF46DA61F1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{673EC5E2-F8C7-4324-B802-271629527E99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14130" yWindow="30" windowWidth="14670" windowHeight="15570" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Teensy 3.6" sheetId="1" r:id="rId1"/>
@@ -73,21 +73,6 @@
     <t>RX3</t>
   </si>
   <si>
-    <t>RX2</t>
-  </si>
-  <si>
-    <t>TX3 (AX12)</t>
-  </si>
-  <si>
-    <t>TX2 (XL320)</t>
-  </si>
-  <si>
-    <t>RX1 (Lidar)</t>
-  </si>
-  <si>
-    <t>TX1 (Lidar)</t>
-  </si>
-  <si>
     <t>DIR_G</t>
   </si>
   <si>
@@ -97,22 +82,37 @@
     <t>DIR_D</t>
   </si>
   <si>
-    <t>RX5</t>
-  </si>
-  <si>
-    <t>TX5</t>
-  </si>
-  <si>
-    <t>RX4</t>
-  </si>
-  <si>
-    <t>TX4</t>
-  </si>
-  <si>
     <t>SCL0</t>
   </si>
   <si>
     <t>SDA0</t>
+  </si>
+  <si>
+    <t>TX3</t>
+  </si>
+  <si>
+    <t>IRQ</t>
+  </si>
+  <si>
+    <t>CE</t>
+  </si>
+  <si>
+    <t>RX2 (Lidar)</t>
+  </si>
+  <si>
+    <t>TX2 (Lidar)</t>
+  </si>
+  <si>
+    <t>MOSI1</t>
+  </si>
+  <si>
+    <t>MISO1</t>
+  </si>
+  <si>
+    <t>CS1</t>
+  </si>
+  <si>
+    <t>SCK1</t>
   </si>
 </sst>
 </file>
@@ -199,11 +199,11 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -551,7 +551,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -585,7 +585,7 @@
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="9" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -597,24 +597,24 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B4" s="4">
         <v>0</v>
       </c>
-      <c r="C4" s="8"/>
+      <c r="C4" s="9"/>
       <c r="D4" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="B5" s="4">
         <v>1</v>
       </c>
-      <c r="C5" s="8"/>
+      <c r="C5" s="9"/>
       <c r="D5" s="4" t="s">
         <v>8</v>
       </c>
@@ -623,7 +623,7 @@
       <c r="B6" s="4">
         <v>2</v>
       </c>
-      <c r="C6" s="8"/>
+      <c r="C6" s="9"/>
       <c r="D6" s="4">
         <v>23</v>
       </c>
@@ -635,11 +635,11 @@
       <c r="B7" s="4">
         <v>3</v>
       </c>
-      <c r="C7" s="8"/>
+      <c r="C7" s="9"/>
       <c r="D7" s="4">
         <v>22</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="8">
         <v>22</v>
       </c>
     </row>
@@ -647,11 +647,11 @@
       <c r="B8" s="4">
         <v>4</v>
       </c>
-      <c r="C8" s="8"/>
+      <c r="C8" s="9"/>
       <c r="D8" s="4">
         <v>21</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="8">
         <v>21</v>
       </c>
     </row>
@@ -659,11 +659,11 @@
       <c r="B9" s="4">
         <v>5</v>
       </c>
-      <c r="C9" s="8"/>
+      <c r="C9" s="9"/>
       <c r="D9" s="4">
         <v>20</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="8">
         <v>20</v>
       </c>
     </row>
@@ -671,12 +671,12 @@
       <c r="B10" s="4">
         <v>6</v>
       </c>
-      <c r="C10" s="8"/>
+      <c r="C10" s="9"/>
       <c r="D10" s="4">
         <v>19</v>
       </c>
-      <c r="E10" s="9" t="s">
-        <v>27</v>
+      <c r="E10" s="8" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -686,76 +686,71 @@
       <c r="B11" s="4">
         <v>7</v>
       </c>
-      <c r="C11" s="8"/>
+      <c r="C11" s="9"/>
       <c r="D11" s="4">
         <v>18</v>
       </c>
-      <c r="E11" s="9" t="s">
-        <v>28</v>
+      <c r="E11" s="8" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="B12" s="4">
         <v>8</v>
       </c>
-      <c r="C12" s="8"/>
+      <c r="C12" s="9"/>
       <c r="D12" s="4">
         <v>17</v>
       </c>
-      <c r="E12" s="9">
-        <v>17</v>
-      </c>
+      <c r="E12" s="8"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="B13" s="4">
         <v>9</v>
       </c>
-      <c r="C13" s="8"/>
+      <c r="C13" s="9"/>
       <c r="D13" s="4">
         <v>16</v>
       </c>
-      <c r="E13" s="9">
-        <v>16</v>
-      </c>
+      <c r="E13" s="8"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B14" s="4">
         <v>10</v>
       </c>
-      <c r="C14" s="8"/>
+      <c r="C14" s="9"/>
       <c r="D14" s="4">
         <v>15</v>
       </c>
-      <c r="E14" s="9">
-        <v>15</v>
-      </c>
+      <c r="E14" s="8"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="4">
         <v>11</v>
       </c>
-      <c r="C15" s="8"/>
+      <c r="C15" s="9"/>
       <c r="D15" s="4">
         <v>14</v>
       </c>
-      <c r="E15" s="9">
-        <v>14</v>
-      </c>
+      <c r="E15" s="8"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
       <c r="B16" s="4">
         <v>12</v>
       </c>
-      <c r="C16" s="8"/>
+      <c r="C16" s="9"/>
       <c r="D16" s="4">
         <v>13</v>
       </c>
@@ -770,7 +765,7 @@
       <c r="B17" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="8"/>
+      <c r="C17" s="9"/>
       <c r="D17" s="4" t="s">
         <v>4</v>
       </c>
@@ -779,10 +774,13 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>21</v>
+      </c>
       <c r="B18" s="4">
         <v>24</v>
       </c>
-      <c r="C18" s="8"/>
+      <c r="C18" s="9"/>
       <c r="D18" s="4" t="s">
         <v>11</v>
       </c>
@@ -791,7 +789,7 @@
       <c r="B19" s="4">
         <v>25</v>
       </c>
-      <c r="C19" s="8"/>
+      <c r="C19" s="9"/>
       <c r="D19" s="4" t="s">
         <v>3</v>
       </c>
@@ -800,19 +798,19 @@
       <c r="B20" s="4">
         <v>26</v>
       </c>
-      <c r="C20" s="8"/>
+      <c r="C20" s="9"/>
       <c r="D20" s="4">
         <v>39</v>
       </c>
       <c r="E20" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" s="4">
         <v>27</v>
       </c>
-      <c r="C21" s="8"/>
+      <c r="C21" s="9"/>
       <c r="D21" s="4">
         <v>38</v>
       </c>
@@ -824,31 +822,31 @@
       <c r="B22" s="4">
         <v>28</v>
       </c>
-      <c r="C22" s="8"/>
+      <c r="C22" s="9"/>
       <c r="D22" s="4">
         <v>37</v>
       </c>
       <c r="E22" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" s="4">
         <v>29</v>
       </c>
-      <c r="C23" s="8"/>
+      <c r="C23" s="9"/>
       <c r="D23" s="4">
         <v>36</v>
       </c>
       <c r="E23" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" s="4">
         <v>30</v>
       </c>
-      <c r="C24" s="8"/>
+      <c r="C24" s="9"/>
       <c r="D24" s="4">
         <v>35</v>
       </c>
@@ -858,32 +856,26 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B25" s="4">
         <v>31</v>
       </c>
-      <c r="C25" s="8"/>
+      <c r="C25" s="9"/>
       <c r="D25" s="4">
         <v>34</v>
       </c>
-      <c r="E25" t="s">
-        <v>23</v>
-      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B26" s="4">
         <v>32</v>
       </c>
-      <c r="C26" s="8"/>
+      <c r="C26" s="9"/>
       <c r="D26" s="4">
         <v>33</v>
-      </c>
-      <c r="E26" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modif elec + modif bom
</commit_message>
<xml_diff>
--- a/Electronique/Carte Robot (base sur un Teensy 3.6)/Brochage Teensy 3.6.xlsx
+++ b/Electronique/Carte Robot (base sur un Teensy 3.6)/Brochage Teensy 3.6.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git folder\my_robot\Electronique\Carte Robot (base sur un Teensy 3.6)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4151757A-73D1-4898-89A9-40061A3AF523}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC4DDFB8-9F67-45E1-848F-36C773C02AD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14130" yWindow="30" windowWidth="14670" windowHeight="15570" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-510" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Brochage PCB" sheetId="2" r:id="rId1"/>
+    <sheet name="Brochage v1" sheetId="2" r:id="rId1"/>
+    <sheet name="Brochage v2" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="51">
   <si>
     <t>Labels</t>
   </si>
@@ -130,6 +131,54 @@
   </si>
   <si>
     <t>CAN0RX</t>
+  </si>
+  <si>
+    <t>LED3</t>
+  </si>
+  <si>
+    <t>LED2</t>
+  </si>
+  <si>
+    <t>RX1 (Lidar)</t>
+  </si>
+  <si>
+    <t>TX1 (Lidar)</t>
+  </si>
+  <si>
+    <t>MOSI0</t>
+  </si>
+  <si>
+    <t>MISO0</t>
+  </si>
+  <si>
+    <t>RX4 (IHM)</t>
+  </si>
+  <si>
+    <t>SCK0</t>
+  </si>
+  <si>
+    <t>CS0</t>
+  </si>
+  <si>
+    <t>TX4 (IHM)</t>
+  </si>
+  <si>
+    <t>TX3 (Act.)</t>
+  </si>
+  <si>
+    <t>RX3 (Act.)</t>
+  </si>
+  <si>
+    <t>SCL2</t>
+  </si>
+  <si>
+    <t>SDA2</t>
+  </si>
+  <si>
+    <t>PWM</t>
+  </si>
+  <si>
+    <t>Microswitch</t>
   </si>
 </sst>
 </file>
@@ -162,12 +211,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -186,6 +236,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -199,7 +261,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -215,8 +277,20 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -275,6 +349,54 @@
       <xdr:spPr>
         <a:xfrm rot="5400000">
           <a:off x="5431339" y="-151768"/>
+          <a:ext cx="4635857" cy="5619750"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>13607</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>149678</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>299357</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>23035</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Image 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C801A787-5229-4567-BFAE-8D964C37B254}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:srcRect r="3870"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="5416371" y="-151768"/>
           <a:ext cx="4635857" cy="5619750"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -552,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE46DD2A-558F-4BCF-AF33-60DC5A92DC6E}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,7 +709,7 @@
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="15" t="s">
         <v>1</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -604,7 +726,7 @@
       <c r="B4" s="4">
         <v>0</v>
       </c>
-      <c r="C4" s="9"/>
+      <c r="C4" s="15"/>
       <c r="D4" s="4" t="s">
         <v>9</v>
       </c>
@@ -616,7 +738,7 @@
       <c r="B5" s="4">
         <v>1</v>
       </c>
-      <c r="C5" s="9"/>
+      <c r="C5" s="15"/>
       <c r="D5" s="4" t="s">
         <v>8</v>
       </c>
@@ -625,7 +747,7 @@
       <c r="B6" s="4">
         <v>2</v>
       </c>
-      <c r="C6" s="9"/>
+      <c r="C6" s="15"/>
       <c r="D6" s="4">
         <v>23</v>
       </c>
@@ -640,11 +762,11 @@
       <c r="B7" s="4">
         <v>3</v>
       </c>
-      <c r="C7" s="9"/>
+      <c r="C7" s="15"/>
       <c r="D7" s="4">
         <v>22</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="7">
         <v>22</v>
       </c>
     </row>
@@ -655,11 +777,11 @@
       <c r="B8" s="4">
         <v>4</v>
       </c>
-      <c r="C8" s="9"/>
+      <c r="C8" s="15"/>
       <c r="D8" s="4">
         <v>21</v>
       </c>
-      <c r="E8" s="8">
+      <c r="E8" s="7">
         <v>21</v>
       </c>
     </row>
@@ -667,11 +789,11 @@
       <c r="B9" s="4">
         <v>5</v>
       </c>
-      <c r="C9" s="9"/>
+      <c r="C9" s="15"/>
       <c r="D9" s="4">
         <v>20</v>
       </c>
-      <c r="E9" s="8">
+      <c r="E9" s="7">
         <v>20</v>
       </c>
     </row>
@@ -679,11 +801,11 @@
       <c r="B10" s="4">
         <v>6</v>
       </c>
-      <c r="C10" s="9"/>
+      <c r="C10" s="15"/>
       <c r="D10" s="4">
         <v>19</v>
       </c>
-      <c r="E10" s="8" t="s">
+      <c r="E10" s="7" t="s">
         <v>18</v>
       </c>
     </row>
@@ -694,11 +816,11 @@
       <c r="B11" s="4">
         <v>7</v>
       </c>
-      <c r="C11" s="9"/>
+      <c r="C11" s="15"/>
       <c r="D11" s="4">
         <v>18</v>
       </c>
-      <c r="E11" s="8" t="s">
+      <c r="E11" s="7" t="s">
         <v>19</v>
       </c>
     </row>
@@ -709,11 +831,13 @@
       <c r="B12" s="4">
         <v>8</v>
       </c>
-      <c r="C12" s="9"/>
+      <c r="C12" s="15"/>
       <c r="D12" s="4">
         <v>17</v>
       </c>
-      <c r="E12" s="8"/>
+      <c r="E12" s="7">
+        <v>17</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -722,11 +846,13 @@
       <c r="B13" s="4">
         <v>9</v>
       </c>
-      <c r="C13" s="9"/>
+      <c r="C13" s="15"/>
       <c r="D13" s="4">
         <v>16</v>
       </c>
-      <c r="E13" s="8"/>
+      <c r="E13" s="7">
+        <v>16</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -735,21 +861,25 @@
       <c r="B14" s="4">
         <v>10</v>
       </c>
-      <c r="C14" s="9"/>
+      <c r="C14" s="15"/>
       <c r="D14" s="4">
         <v>15</v>
       </c>
-      <c r="E14" s="8"/>
+      <c r="E14" s="7">
+        <v>15</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="4">
         <v>11</v>
       </c>
-      <c r="C15" s="9"/>
+      <c r="C15" s="15"/>
       <c r="D15" s="4">
         <v>14</v>
       </c>
-      <c r="E15" s="8"/>
+      <c r="E15" s="7">
+        <v>14</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -758,11 +888,11 @@
       <c r="B16" s="4">
         <v>12</v>
       </c>
-      <c r="C16" s="9"/>
+      <c r="C16" s="15"/>
       <c r="D16" s="4">
         <v>13</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="E16" s="8" t="s">
         <v>10</v>
       </c>
     </row>
@@ -773,7 +903,7 @@
       <c r="B17" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="9"/>
+      <c r="C17" s="15"/>
       <c r="D17" s="4" t="s">
         <v>4</v>
       </c>
@@ -788,25 +918,31 @@
       <c r="B18" s="4">
         <v>24</v>
       </c>
-      <c r="C18" s="9"/>
+      <c r="C18" s="15"/>
       <c r="D18" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>36</v>
+      </c>
       <c r="B19" s="4">
         <v>25</v>
       </c>
-      <c r="C19" s="9"/>
+      <c r="C19" s="15"/>
       <c r="D19" s="4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
       <c r="B20" s="4">
         <v>26</v>
       </c>
-      <c r="C20" s="9"/>
+      <c r="C20" s="15"/>
       <c r="D20" s="4">
         <v>39</v>
       </c>
@@ -821,7 +957,7 @@
       <c r="B21" s="4">
         <v>27</v>
       </c>
-      <c r="C21" s="9"/>
+      <c r="C21" s="15"/>
       <c r="D21" s="4">
         <v>38</v>
       </c>
@@ -836,7 +972,7 @@
       <c r="B22" s="4">
         <v>28</v>
       </c>
-      <c r="C22" s="9"/>
+      <c r="C22" s="15"/>
       <c r="D22" s="4">
         <v>37</v>
       </c>
@@ -851,7 +987,7 @@
       <c r="B23" s="4">
         <v>29</v>
       </c>
-      <c r="C23" s="9"/>
+      <c r="C23" s="15"/>
       <c r="D23" s="4">
         <v>36</v>
       </c>
@@ -866,7 +1002,7 @@
       <c r="B24" s="4">
         <v>30</v>
       </c>
-      <c r="C24" s="9"/>
+      <c r="C24" s="15"/>
       <c r="D24" s="4">
         <v>35</v>
       </c>
@@ -881,7 +1017,7 @@
       <c r="B25" s="4">
         <v>31</v>
       </c>
-      <c r="C25" s="9"/>
+      <c r="C25" s="15"/>
       <c r="D25" s="4">
         <v>34</v>
       </c>
@@ -893,10 +1029,386 @@
       <c r="B26" s="4">
         <v>32</v>
       </c>
-      <c r="C26" s="9"/>
+      <c r="C26" s="15"/>
       <c r="D26" s="4">
         <v>33</v>
       </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C3:C26"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{508AD10A-4EA1-48EB-B49F-EEA08DF4CCAB}">
+  <dimension ref="A1:E26"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="10.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="15.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="2"/>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="4">
+        <v>0</v>
+      </c>
+      <c r="C4" s="15"/>
+      <c r="D4" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="15"/>
+      <c r="D5" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="12"/>
+      <c r="B6" s="4">
+        <v>2</v>
+      </c>
+      <c r="C6" s="15"/>
+      <c r="D6" s="4">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="4">
+        <v>3</v>
+      </c>
+      <c r="C7" s="15"/>
+      <c r="D7" s="4">
+        <v>22</v>
+      </c>
+      <c r="E7" s="13"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="4">
+        <v>4</v>
+      </c>
+      <c r="C8" s="15"/>
+      <c r="D8" s="4">
+        <v>21</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="12"/>
+      <c r="B9" s="4">
+        <v>5</v>
+      </c>
+      <c r="C9" s="15"/>
+      <c r="D9" s="4">
+        <v>20</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="12"/>
+      <c r="B10" s="4">
+        <v>6</v>
+      </c>
+      <c r="C10" s="15"/>
+      <c r="D10" s="4">
+        <v>19</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="4">
+        <v>7</v>
+      </c>
+      <c r="C11" s="15"/>
+      <c r="D11" s="4">
+        <v>18</v>
+      </c>
+      <c r="E11" s="11" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="4">
+        <v>8</v>
+      </c>
+      <c r="C12" s="15"/>
+      <c r="D12" s="4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" s="4">
+        <v>9</v>
+      </c>
+      <c r="C13" s="15"/>
+      <c r="D13" s="4">
+        <v>16</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="4">
+        <v>10</v>
+      </c>
+      <c r="C14" s="15"/>
+      <c r="D14" s="4">
+        <v>15</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="4">
+        <v>11</v>
+      </c>
+      <c r="C15" s="15"/>
+      <c r="D15" s="4">
+        <v>14</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B16" s="4">
+        <v>12</v>
+      </c>
+      <c r="C16" s="15"/>
+      <c r="D16" s="4">
+        <v>13</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C17" s="15"/>
+      <c r="D17" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" s="4">
+        <v>24</v>
+      </c>
+      <c r="C18" s="15"/>
+      <c r="D18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="14"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>32</v>
+      </c>
+      <c r="B19" s="4">
+        <v>25</v>
+      </c>
+      <c r="C19" s="15"/>
+      <c r="D19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E19" s="14"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="4">
+        <v>26</v>
+      </c>
+      <c r="C20" s="15"/>
+      <c r="D20" s="4">
+        <v>39</v>
+      </c>
+      <c r="E20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" s="4">
+        <v>27</v>
+      </c>
+      <c r="C21" s="15"/>
+      <c r="D21" s="4">
+        <v>38</v>
+      </c>
+      <c r="E21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" s="4">
+        <v>28</v>
+      </c>
+      <c r="C22" s="15"/>
+      <c r="D22" s="4">
+        <v>37</v>
+      </c>
+      <c r="E22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="4">
+        <v>29</v>
+      </c>
+      <c r="C23" s="15"/>
+      <c r="D23" s="4">
+        <v>36</v>
+      </c>
+      <c r="E23" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" s="4">
+        <v>30</v>
+      </c>
+      <c r="C24" s="15"/>
+      <c r="D24" s="4">
+        <v>35</v>
+      </c>
+      <c r="E24" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>41</v>
+      </c>
+      <c r="B25" s="4">
+        <v>31</v>
+      </c>
+      <c r="C25" s="15"/>
+      <c r="D25" s="4">
+        <v>34</v>
+      </c>
+      <c r="E25" s="13"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B26" s="4">
+        <v>32</v>
+      </c>
+      <c r="C26" s="15"/>
+      <c r="D26" s="4">
+        <v>33</v>
+      </c>
+      <c r="E26" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>